<commit_message>
add somenumber in cs.xlsz
</commit_message>
<xml_diff>
--- a/cs.xlsx
+++ b/cs.xlsx
@@ -357,22 +357,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
+      <c r="B1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>